<commit_message>
Complete working prototype Only thing to remove is _x000c_
</commit_message>
<xml_diff>
--- a/GridCSVs/Data_Extraction01.xlsx
+++ b/GridCSVs/Data_Extraction01.xlsx
@@ -31,16 +31,16 @@
     <t>E-Mail</t>
   </si>
   <si>
-    <t xml:space="preserve">Invoice Number INV-3337 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">From: DEMO Sliced Invoices Suite 5A-1204 123 Somewhere Street Your City AZ 12345 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To: Test Business 123 Somewhere St Melbourne; VIC 3000 tocttoct Con </t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin@slicedinvoices, </t>
+    <t xml:space="preserve">Invoice Number INV-333 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">From: DEMO Sliced Invoices Suite 5A-1204 123 Somewhere Street Your Citv 4Z 12345 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To: Test Business 123 Somewhere St Melbourne, VIC 3000 testtest com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">test@test, admin@slicedinvoices, </t>
   </si>
 </sst>
 </file>

</xml_diff>